<commit_message>
corrected income tax and median home price files
</commit_message>
<xml_diff>
--- a/state_income_tax.xlsx
+++ b/state_income_tax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\2. Group_Project_1\SMUDS-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFFA674-FF51-4BDF-9349-6AC441B55079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2B3ED-1299-4A63-9F97-D3D3FD992A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="15048" windowHeight="10956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Highest Marginal income tax rate 2019 (%)</t>
-  </si>
-  <si>
     <t>AL</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>DC</t>
+  </si>
+  <si>
+    <t>Highest Marginal Income Tax Rate (%)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -512,13 +512,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>5</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>4.54</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>6.9</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>12.3</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>4.63</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>6.99</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>6.6</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>5.75</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>11</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>6.9249999999999998</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>4.95</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>3.23</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>8.5299999999999994</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>5.7</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5">
         <v>5</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>6</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5">
         <v>7.15</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>5.75</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>5.05</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>4.25</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>9.85</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>5</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5">
         <v>5.4</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>6.9</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5">
         <v>6.84</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5">
         <v>0</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>10.75</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="5">
         <v>4.9000000000000004</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>8.82</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="5">
         <v>5.25</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="5">
         <v>2.9</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5">
         <v>4.9969999999999999</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5">
         <v>5</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="5">
         <v>9.9</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5">
         <v>3.07</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5">
         <v>5.99</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5">
         <v>7</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="5">
         <v>0</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="5">
         <v>0</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5">
         <v>4.95</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5">
         <v>8.75</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="5">
         <v>5.75</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5">
         <v>6.5</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="5">
         <v>7.65</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="5">
         <v>0</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="5">
         <v>8.9499999999999993</v>

</xml_diff>